<commit_message>
understanfd the varience of data
</commit_message>
<xml_diff>
--- a/varience.xlsx
+++ b/varience.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8837BDEF-FA21-4DB8-8004-3F97F24F707C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B509DA78-04E7-4221-81FD-BD8E5E77F810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{97F130BB-D129-449A-B928-3283440F0F04}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="21600" windowHeight="11772" xr2:uid="{97F130BB-D129-449A-B928-3283440F0F04}"/>
   </bookViews>
   <sheets>
     <sheet name="varience" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>🎓 Example: 2 Students with same average, but different variance</t>
   </si>
@@ -55,6 +55,33 @@
   </si>
   <si>
     <t>(xi - m)2</t>
+  </si>
+  <si>
+    <t>Élève</t>
+  </si>
+  <si>
+    <t>Classe A</t>
+  </si>
+  <si>
+    <t>Classe B</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>xi - avg</t>
+  </si>
+  <si>
+    <t>Somme</t>
+  </si>
+  <si>
+    <t>(xi - avg)2</t>
+  </si>
+  <si>
+    <t>moy</t>
+  </si>
+  <si>
+    <t>varPop</t>
   </si>
 </sst>
 </file>
@@ -86,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,8 +144,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -154,15 +199,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -185,6 +264,52 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2335,209 +2460,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6381475D-C75F-4056-9B19-3C1F3BA65496}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>10</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>15</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <f>C11-$C$15</f>
         <v>0</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <f>POWER(E11,2)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f>D11-$D$15</f>
         <v>5</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f>POWER(G11,2)</f>
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>10</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>15</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <f t="shared" ref="E12:E14" si="0">C12-$C$15</f>
         <v>0</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <f t="shared" ref="F12:F14" si="1">POWER(E12,2)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <f t="shared" ref="G12:G14" si="2">D12-$D$15</f>
         <v>5</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <f t="shared" ref="H12:H14" si="3">POWER(G12,2)</f>
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>10</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>9</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>10</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>1</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <f t="shared" si="2"/>
         <v>-9</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <f t="shared" si="3"/>
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <f>AVERAGE(C11:C14)</f>
         <v>10</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f>AVERAGE(D11:D14)</f>
         <v>10</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <f>_xlfn.VAR.S(C11:C14)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <f>_xlfn.VAR.S(D11:D14)</f>
         <v>44</v>
       </c>
@@ -2558,9 +2683,209 @@
         <v>44</v>
       </c>
     </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F40" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="25"/>
+      <c r="J40" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J41" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="11">
+        <v>1</v>
+      </c>
+      <c r="B42" s="16">
+        <v>10</v>
+      </c>
+      <c r="C42" s="18">
+        <v>6</v>
+      </c>
+      <c r="E42" s="22">
+        <v>1</v>
+      </c>
+      <c r="F42" s="23">
+        <f>B42-$B$46</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="24">
+        <f>C42-$C$46</f>
+        <v>-4</v>
+      </c>
+      <c r="I42" s="22">
+        <v>1</v>
+      </c>
+      <c r="J42" s="23">
+        <f>POWER(F42,2)</f>
+        <v>0</v>
+      </c>
+      <c r="K42" s="24">
+        <f>POWER(G42,2)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="11">
+        <v>2</v>
+      </c>
+      <c r="B43" s="16">
+        <v>10</v>
+      </c>
+      <c r="C43" s="18">
+        <v>10</v>
+      </c>
+      <c r="E43" s="22">
+        <v>2</v>
+      </c>
+      <c r="F43" s="23">
+        <f t="shared" ref="F43:F44" si="4">B43-$B$46</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="24">
+        <f t="shared" ref="G43:G44" si="5">C43-$C$46</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="22">
+        <v>2</v>
+      </c>
+      <c r="J43" s="23">
+        <f t="shared" ref="J43:J44" si="6">POWER(F43,2)</f>
+        <v>0</v>
+      </c>
+      <c r="K43" s="24">
+        <f t="shared" ref="K43:K44" si="7">POWER(G43,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="11">
+        <v>3</v>
+      </c>
+      <c r="B44" s="16">
+        <v>10</v>
+      </c>
+      <c r="C44" s="18">
+        <v>14</v>
+      </c>
+      <c r="E44" s="22">
+        <v>3</v>
+      </c>
+      <c r="F44" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G44" s="24">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="I44" s="22">
+        <v>3</v>
+      </c>
+      <c r="J44" s="23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="24">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="13">
+        <f>AVERAGE(B42:B44)</f>
+        <v>10</v>
+      </c>
+      <c r="C46" s="14">
+        <f>AVERAGE(C42:C44)</f>
+        <v>10</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="13">
+        <f>SUM(F42:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="14">
+        <f>SUM(G42:G44)</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="13">
+        <f>SUM(J42:J44)</f>
+        <v>0</v>
+      </c>
+      <c r="K46" s="14">
+        <f>SUM(K42:K44)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="9:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="9:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I51" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="13">
+        <f>J46/3</f>
+        <v>0</v>
+      </c>
+      <c r="K51" s="14">
+        <f>K46/3</f>
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="53" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="J53" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="K53" s="26">
+        <f>_xlfn.VAR.P(C42:C44)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="L53" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:F6"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="J40:K40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>